<commit_message>
updated the rubric and meeting notes
</commit_message>
<xml_diff>
--- a/Project Documentation/Game Team Progression Rubric.xlsx
+++ b/Project Documentation/Game Team Progression Rubric.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEV4_HANDOUT\Project Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\dev4-team-project-2404-blue-team-2404\Project Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD757B81-3B40-4DD3-9469-957C3698E417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5FBCC5-95B5-4AB8-9E82-7FDDFEEF687F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-14510" windowWidth="34620" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team Info" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="104">
   <si>
     <t>Team Code Name</t>
   </si>
@@ -166,9 +166,6 @@
     <t>John Doe</t>
   </si>
   <si>
-    <t>Joe Public</t>
-  </si>
-  <si>
     <t>Joe Bloggs</t>
   </si>
   <si>
@@ -187,30 +184,9 @@
     <t>Pitfall - https://youtu.be/l_lJ-ONcMEs</t>
   </si>
   <si>
-    <t>Monday 3pm-5pm - Weekly/Sprint planning</t>
-  </si>
-  <si>
-    <t>https://our_team_repo.git</t>
-  </si>
-  <si>
-    <t>Tuesday 11am-11:15am - Daily standup meeting</t>
-  </si>
-  <si>
-    <t>Wednsday 2pm-3pm - Code merge confrence call</t>
-  </si>
-  <si>
-    <t>Thursday 11am-11:15am - Daily standup meeting</t>
-  </si>
-  <si>
-    <t>Friday 4pm-6pm - Build/Release candidate testing</t>
-  </si>
-  <si>
     <t>Jira Project URL</t>
   </si>
   <si>
-    <t>https://ourgameproject.atlassian.net/jira/your-work</t>
-  </si>
-  <si>
     <t>Instructors Invited To Jira (Yes/No)</t>
   </si>
   <si>
@@ -442,9 +418,6 @@
     <t>Gameplay Programmer, Secondary Lead</t>
   </si>
   <si>
-    <t>Graphics Programmer, Secondary Gameplay</t>
-  </si>
-  <si>
     <t>Generalist Programmer, Secondary Gameplay</t>
   </si>
   <si>
@@ -458,6 +431,30 @@
   </si>
   <si>
     <t>Game Mechanics Based On:</t>
+  </si>
+  <si>
+    <t>Saturday 1:00 pm est - Sprint planning (after 1st week)</t>
+  </si>
+  <si>
+    <t>Monday 7 pm est - project planning (1st week) / Daily Standup meeting</t>
+  </si>
+  <si>
+    <t>Thursday 7 pm est - Code Merge conference call</t>
+  </si>
+  <si>
+    <t>Friday 6pm est - final build conference test</t>
+  </si>
+  <si>
+    <t>Wednsday 7 pm est - Daily Standup meeting</t>
+  </si>
+  <si>
+    <t>https://github.com/orgs/FSProjectPortfolioIV/teams/blue-team-2404</t>
+  </si>
+  <si>
+    <t>Andrew Sipes</t>
+  </si>
+  <si>
+    <t>Graphics Programmer, Secondary Lead</t>
   </si>
 </sst>
 </file>
@@ -931,7 +928,7 @@
     <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="6"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="5" applyBorder="1"/>
@@ -980,10 +977,7 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="4" xfId="12" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="4" xfId="11" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1010,52 +1004,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Warning Text" xfId="8" builtinId="11"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <b/>
@@ -1467,16 +1416,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="50.7265625" customWidth="1"/>
+    <col min="1" max="2" width="50.7109375" customWidth="1"/>
+    <col min="3" max="3" width="68.85546875" customWidth="1"/>
+    <col min="4" max="4" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1490,9 +1441,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
@@ -1501,122 +1452,110 @@
         <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C5" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="D5" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" s="6"/>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" s="12"/>
       <c r="D7" s="13"/>
     </row>
-    <row r="8" spans="1:4" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="C8" s="11" t="s">
+      <c r="D8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="14" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
+      <c r="B9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="C9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D16" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="15" t="s">
+    </row>
+    <row r="17" spans="4:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="24"/>
+    </row>
+    <row r="19" spans="4:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D19" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="9" t="s">
+    </row>
+    <row r="20" spans="4:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C10" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C11" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C12" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C13" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D16" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="D17" s="24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D19" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="4:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="D20" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1" xr:uid="{C667DB4A-0C6F-4AD2-88BD-A7EED763DC9F}"/>
-    <hyperlink ref="D17" r:id="rId2" xr:uid="{274D2EFD-F288-4087-98D9-4511BEC7387B}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1624,694 +1563,694 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976D0730-B5D0-49E5-8631-8CC13B9FE765}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A35" sqref="A32:A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="83.453125" customWidth="1"/>
-    <col min="2" max="3" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.81640625" customWidth="1"/>
-    <col min="11" max="12" width="13.81640625" customWidth="1"/>
+    <col min="1" max="1" width="83.42578125" customWidth="1"/>
+    <col min="2" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="11" max="12" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="23" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="L1" s="25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="36" t="s">
-        <v>29</v>
+        <v>20</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C2" s="21">
         <v>-100</v>
       </c>
       <c r="K2" s="28" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="L2" s="28" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="36" t="s">
-        <v>29</v>
+        <v>23</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C3" s="22">
         <v>-75</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="L3" s="30" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="36" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C4" s="21">
         <v>-50</v>
       </c>
       <c r="K4" s="27" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="L4" s="26" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C5" s="21">
         <v>-45</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="36" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C6" s="21">
         <v>-40</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="36" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C7" s="21">
         <v>-37</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="36" t="s">
         <v>29</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C8" s="21">
         <v>-35</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="36" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C9" s="21">
         <v>-25</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="36" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C10" s="21">
         <v>-20</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="B11" s="36" t="s">
-        <v>29</v>
+        <v>88</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C11" s="21">
         <v>-15</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="36" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C12" s="21">
         <v>-15</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="36" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C13" s="21">
         <v>-15</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="36" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C14" s="21">
         <v>-15</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="36" t="s">
-        <v>29</v>
+        <v>35</v>
+      </c>
+      <c r="B15" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C15" s="21">
         <v>-15</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="36" t="s">
-        <v>29</v>
+        <v>36</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C16" s="21">
         <v>-15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="36" t="s">
-        <v>29</v>
+        <v>37</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C17" s="21">
         <v>-12</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="36" t="s">
-        <v>29</v>
+        <v>38</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C18" s="21">
         <v>-12</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="36" t="s">
-        <v>29</v>
+        <v>39</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C19" s="21">
         <v>-10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="B20" s="36" t="s">
-        <v>29</v>
+        <v>85</v>
+      </c>
+      <c r="B20" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C20" s="21">
         <v>-10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="B21" s="36" t="s">
-        <v>29</v>
+        <v>86</v>
+      </c>
+      <c r="B21" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C21" s="21">
         <v>-10</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" s="36" t="s">
-        <v>29</v>
+        <v>87</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C22" s="21">
         <v>-10</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="36" t="s">
-        <v>29</v>
+        <v>40</v>
+      </c>
+      <c r="B23" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C23" s="21">
         <v>-8</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="36" t="s">
-        <v>29</v>
+        <v>41</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C24" s="21">
         <v>-8</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="36" t="s">
-        <v>29</v>
+        <v>42</v>
+      </c>
+      <c r="B25" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C25" s="21">
         <v>-8</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="36" t="s">
-        <v>29</v>
+        <v>43</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C26" s="21">
         <v>-6</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="36" t="s">
-        <v>29</v>
+        <v>44</v>
+      </c>
+      <c r="B27" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C27" s="21">
         <v>-6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="36" t="s">
-        <v>29</v>
+        <v>45</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C28" s="21">
         <v>-6</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="B29" s="36" t="s">
-        <v>29</v>
+        <v>84</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C29" s="21">
         <v>-6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="36" t="s">
-        <v>29</v>
+        <v>46</v>
+      </c>
+      <c r="B30" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C30" s="21">
         <v>-5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="36" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="B31" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C31" s="21">
         <v>-5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="B32" s="36" t="s">
-        <v>29</v>
+        <v>59</v>
+      </c>
+      <c r="B32" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C32" s="21">
         <v>-3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="B33" s="36" t="s">
-        <v>29</v>
+        <v>48</v>
+      </c>
+      <c r="B33" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C33" s="21">
         <v>-3</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="B34" s="36" t="s">
-        <v>29</v>
+        <v>49</v>
+      </c>
+      <c r="B34" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C34" s="21">
         <v>-2</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" s="36" t="s">
-        <v>29</v>
+        <v>50</v>
+      </c>
+      <c r="B35" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C35" s="21">
         <v>-2</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="B36" s="34">
+    <row r="36" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="23">
         <f>100+SUMPRODUCT(SUMIF($B$2:$B$35,$K$4,$C$2:$C$35))+SUMPRODUCT(SUMIF($B$2:$B$35,$K$3,$C$2:$C$35))*0.5</f>
         <v>-549</v>
       </c>
-      <c r="C36" s="35">
+      <c r="C36" s="34">
         <f>SUMPRODUCT(SUMIF($B$2:$B$35,$K$4,$C$2:$C$35))+SUMPRODUCT(SUMIF($B$2:$B$35,$K$3,$C$2:$C$35))*0.5</f>
         <v>-649</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="20"/>
       <c r="B37" s="19"/>
       <c r="C37" s="19"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" s="19"/>
       <c r="C38" s="19"/>
     </row>
-    <row r="39" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="39" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="23" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A40" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="B40" s="36" t="s">
-        <v>79</v>
+        <v>55</v>
+      </c>
+      <c r="B40" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="C40" s="29">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="B41" s="36" t="s">
-        <v>79</v>
+        <v>93</v>
+      </c>
+      <c r="B41" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="C41" s="29">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="B42" s="36" t="s">
-        <v>79</v>
+        <v>94</v>
+      </c>
+      <c r="B42" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="C42" s="29">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="B43" s="36" t="s">
-        <v>79</v>
+        <v>68</v>
+      </c>
+      <c r="B43" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="C43" s="29">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="B44" s="36" t="s">
-        <v>79</v>
+        <v>60</v>
+      </c>
+      <c r="B44" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="C44" s="29">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="B45" s="36" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="B45" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="C45" s="29">
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="B46" s="36" t="s">
         <v>79</v>
+      </c>
+      <c r="B46" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="C46" s="29">
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="B47" s="36" t="s">
-        <v>79</v>
+        <v>56</v>
+      </c>
+      <c r="B47" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="C47" s="29">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="B48" s="36" t="s">
-        <v>79</v>
+        <v>92</v>
+      </c>
+      <c r="B48" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="C48" s="29">
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="B49" s="36" t="s">
-        <v>79</v>
+        <v>61</v>
+      </c>
+      <c r="B49" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="C49" s="29">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="B50" s="36" t="s">
-        <v>79</v>
+        <v>67</v>
+      </c>
+      <c r="B50" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="C50" s="29">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="B51" s="36" t="s">
-        <v>79</v>
+        <v>66</v>
+      </c>
+      <c r="B51" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="C51" s="29">
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="B52" s="36" t="s">
-        <v>79</v>
+        <v>65</v>
+      </c>
+      <c r="B52" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="C52" s="29">
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="B53" s="36" t="s">
-        <v>79</v>
+        <v>64</v>
+      </c>
+      <c r="B53" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="C53" s="29">
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="B54" s="36" t="s">
-        <v>79</v>
+        <v>57</v>
+      </c>
+      <c r="B54" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="C54" s="29">
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B55" s="36" t="s">
-        <v>79</v>
+        <v>58</v>
+      </c>
+      <c r="B55" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="C55" s="29">
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="B56" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="B56" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="C56" s="29">
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="B57" s="36" t="s">
-        <v>79</v>
+        <v>54</v>
+      </c>
+      <c r="B57" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="C57" s="29">
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B58" s="36" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="B58" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="C58" s="29">
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="B59" s="36" t="s">
-        <v>79</v>
+        <v>72</v>
+      </c>
+      <c r="B59" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="C59" s="29">
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="B60" s="36" t="s">
-        <v>79</v>
+        <v>63</v>
+      </c>
+      <c r="B60" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="C60" s="29">
         <v>35</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="61" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="23" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B61" s="23">
         <f>B$36+SUMPRODUCT(SUMIF($B$40:$B$60,$L$1,$C$40:$C$60))+SUMPRODUCT(SUMIF($B$40:$B$60,$L$3,$C$40:$C$60))*0.5</f>
@@ -2322,35 +2261,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="64" spans="1:3" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="18" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B64" s="10"/>
     </row>
-    <row r="65" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B65" s="37" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+      <c r="B65" s="36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B66" s="37" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+      <c r="B66" s="36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B67" s="37" t="s">
-        <v>79</v>
+        <v>81</v>
+      </c>
+      <c r="B67" s="36" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2358,60 +2297,46 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A40:C61">
     <sortCondition ref="C40:C61"/>
   </sortState>
-  <conditionalFormatting sqref="B2:B10 B12:B35">
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+  <conditionalFormatting sqref="B2:B35">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>$K$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>$K$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>$K$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>$K$1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B40:B60 B66:B67">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+  <conditionalFormatting sqref="B40:B60">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>$L$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
       <formula>$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
       <formula>$L$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="12" operator="equal">
       <formula>$L$1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B65">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+  <conditionalFormatting sqref="B65:B67">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>$L$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
       <formula>$L$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
       <formula>$L$1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B11">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>$K$4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>$K$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>$K$2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
-      <formula>$K$1</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">

</xml_diff>

<commit_message>
updated rubric with team info
</commit_message>
<xml_diff>
--- a/Project Documentation/Game Team Progression Rubric.xlsx
+++ b/Project Documentation/Game Team Progression Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\dev4-team-project-2404-blue-team-2404\Project Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5FBCC5-95B5-4AB8-9E82-7FDDFEEF687F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC7A2A9-A365-45CC-B85D-8885FD20801E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-14510" windowWidth="34620" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="106">
   <si>
     <t>Team Code Name</t>
   </si>
@@ -157,18 +157,6 @@
     <t>Team Member Roles</t>
   </si>
   <si>
-    <t>What do you call yourselves?</t>
-  </si>
-  <si>
-    <t>Jane Doe</t>
-  </si>
-  <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>Joe Bloggs</t>
-  </si>
-  <si>
     <t>Game Name</t>
   </si>
   <si>
@@ -181,18 +169,12 @@
     <t>Rope Swinging Crazy Man</t>
   </si>
   <si>
-    <t>Pitfall - https://youtu.be/l_lJ-ONcMEs</t>
-  </si>
-  <si>
     <t>Jira Project URL</t>
   </si>
   <si>
     <t>Instructors Invited To Jira (Yes/No)</t>
   </si>
   <si>
-    <t>Not Yet</t>
-  </si>
-  <si>
     <t>Fully Complete Review Score = 100</t>
   </si>
   <si>
@@ -373,9 +355,6 @@
     <t>The Game's Score After Critic Deductions:</t>
   </si>
   <si>
-    <t>Team-Color?</t>
-  </si>
-  <si>
     <t>Game supports game controller for all features.</t>
   </si>
   <si>
@@ -412,15 +391,6 @@
     <t>The game's levels are missing walls/objects or don't appear as expected.</t>
   </si>
   <si>
-    <t>Lead Programmer, Secondary Graphics</t>
-  </si>
-  <si>
-    <t>Gameplay Programmer, Secondary Lead</t>
-  </si>
-  <si>
-    <t>Generalist Programmer, Secondary Gameplay</t>
-  </si>
-  <si>
     <t>Team has a post-mortem presentation of the game in class on day 8 lecture.</t>
   </si>
   <si>
@@ -455,6 +425,42 @@
   </si>
   <si>
     <t>Graphics Programmer, Secondary Lead</t>
+  </si>
+  <si>
+    <t>https://blueteam2404.atlassian.net/jira/software/c/projects/PP4/boards/3</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Adam Mashaw</t>
+  </si>
+  <si>
+    <t>Sandy Boyett</t>
+  </si>
+  <si>
+    <t>Rafael Vargas</t>
+  </si>
+  <si>
+    <t>James Green</t>
+  </si>
+  <si>
+    <t>Gameplay Programmer, Secondary Generalist</t>
+  </si>
+  <si>
+    <t>Generalist Programmer, Secondary Graphics</t>
+  </si>
+  <si>
+    <t>Lead Programmer, Secondary Gameplay</t>
+  </si>
+  <si>
+    <t>Emberlight</t>
+  </si>
+  <si>
+    <t>Team-Color? Blue 2404</t>
+  </si>
+  <si>
+    <t>Pitfall - https://youtu.be/WSGwL2xznfM</t>
   </si>
 </sst>
 </file>
@@ -1417,14 +1423,14 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="50.7109375" customWidth="1"/>
     <col min="3" max="3" width="68.85546875" customWidth="1"/>
-    <col min="4" max="4" width="50.7109375" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1443,45 +1449,49 @@
     </row>
     <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>5</v>
+        <v>96</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="6"/>
-      <c r="D6" s="7"/>
+      <c r="C6" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" s="12"/>
@@ -1489,73 +1499,78 @@
     </row>
     <row r="8" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>12</v>
+        <v>105</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C13" s="15" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D16" s="14" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="4:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="24"/>
+      <c r="D17" s="24" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="19" spans="4:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D19" s="14" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="4:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D20" s="8" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D17" r:id="rId1" xr:uid="{94AEBCEE-743F-416E-9E82-90E4D7A07704}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1577,78 +1592,78 @@
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="23" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="L1" s="25" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C2" s="21">
         <v>-100</v>
       </c>
       <c r="K2" s="28" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="L2" s="28" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C3" s="22">
         <v>-75</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="L3" s="30" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C4" s="21">
         <v>-50</v>
       </c>
       <c r="K4" s="27" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="L4" s="26" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C5" s="21">
         <v>-45</v>
@@ -1656,10 +1671,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C6" s="21">
         <v>-40</v>
@@ -1667,10 +1682,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C7" s="21">
         <v>-37</v>
@@ -1678,10 +1693,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C8" s="21">
         <v>-35</v>
@@ -1689,10 +1704,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C9" s="21">
         <v>-25</v>
@@ -1700,10 +1715,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C10" s="21">
         <v>-20</v>
@@ -1711,10 +1726,10 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C11" s="21">
         <v>-15</v>
@@ -1722,10 +1737,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C12" s="21">
         <v>-15</v>
@@ -1733,10 +1748,10 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C13" s="21">
         <v>-15</v>
@@ -1744,10 +1759,10 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C14" s="21">
         <v>-15</v>
@@ -1755,10 +1770,10 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B15" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C15" s="21">
         <v>-15</v>
@@ -1766,10 +1781,10 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C16" s="21">
         <v>-15</v>
@@ -1777,10 +1792,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C17" s="21">
         <v>-12</v>
@@ -1788,10 +1803,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C18" s="21">
         <v>-12</v>
@@ -1799,10 +1814,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B19" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C19" s="21">
         <v>-10</v>
@@ -1810,10 +1825,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B20" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C20" s="21">
         <v>-10</v>
@@ -1821,10 +1836,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B21" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C21" s="21">
         <v>-10</v>
@@ -1832,10 +1847,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C22" s="21">
         <v>-10</v>
@@ -1843,10 +1858,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B23" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C23" s="21">
         <v>-8</v>
@@ -1854,10 +1869,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="33" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B24" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C24" s="21">
         <v>-8</v>
@@ -1865,10 +1880,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B25" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C25" s="21">
         <v>-8</v>
@@ -1876,10 +1891,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B26" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C26" s="21">
         <v>-6</v>
@@ -1887,10 +1902,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B27" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C27" s="21">
         <v>-6</v>
@@ -1898,10 +1913,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B28" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C28" s="21">
         <v>-6</v>
@@ -1909,10 +1924,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B29" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C29" s="21">
         <v>-6</v>
@@ -1920,10 +1935,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B30" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C30" s="21">
         <v>-5</v>
@@ -1931,10 +1946,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="33" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B31" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C31" s="21">
         <v>-5</v>
@@ -1942,10 +1957,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="33" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B32" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C32" s="21">
         <v>-3</v>
@@ -1953,10 +1968,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="33" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B33" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C33" s="21">
         <v>-3</v>
@@ -1964,10 +1979,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="33" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B34" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C34" s="21">
         <v>-2</v>
@@ -1975,10 +1990,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="33" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B35" s="35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C35" s="21">
         <v>-2</v>
@@ -1986,7 +2001,7 @@
     </row>
     <row r="36" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="23" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B36" s="23">
         <f>100+SUMPRODUCT(SUMIF($B$2:$B$35,$K$4,$C$2:$C$35))+SUMPRODUCT(SUMIF($B$2:$B$35,$K$3,$C$2:$C$35))*0.5</f>
@@ -2008,21 +2023,21 @@
     </row>
     <row r="39" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="23" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A40" s="32" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B40" s="35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C40" s="29">
         <v>2</v>
@@ -2030,10 +2045,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="32" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B41" s="35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C41" s="29">
         <v>2</v>
@@ -2041,10 +2056,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="32" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B42" s="35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C42" s="29">
         <v>2</v>
@@ -2052,10 +2067,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="32" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B43" s="35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C43" s="29">
         <v>2</v>
@@ -2063,10 +2078,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="32" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B44" s="35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C44" s="29">
         <v>3</v>
@@ -2074,10 +2089,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="32" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B45" s="35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C45" s="29">
         <v>5</v>
@@ -2085,10 +2100,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="32" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B46" s="35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C46" s="29">
         <v>5</v>
@@ -2096,10 +2111,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="32" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B47" s="35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C47" s="29">
         <v>5</v>
@@ -2107,10 +2122,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="32" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B48" s="35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C48" s="29">
         <v>5</v>
@@ -2118,10 +2133,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="32" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B49" s="35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C49" s="29">
         <v>5</v>
@@ -2129,10 +2144,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="32" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B50" s="35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C50" s="29">
         <v>5</v>
@@ -2140,10 +2155,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="32" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B51" s="35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C51" s="29">
         <v>5</v>
@@ -2151,10 +2166,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="32" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B52" s="35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C52" s="29">
         <v>5</v>
@@ -2162,10 +2177,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="32" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B53" s="35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C53" s="29">
         <v>7</v>
@@ -2173,10 +2188,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="32" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B54" s="35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C54" s="29">
         <v>7</v>
@@ -2184,10 +2199,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="32" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B55" s="35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C55" s="29">
         <v>7</v>
@@ -2195,10 +2210,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="32" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B56" s="35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C56" s="29">
         <v>7</v>
@@ -2206,10 +2221,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="32" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B57" s="35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C57" s="29">
         <v>7</v>
@@ -2217,10 +2232,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="32" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B58" s="35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C58" s="29">
         <v>15</v>
@@ -2228,10 +2243,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="32" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B59" s="35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C59" s="29">
         <v>25</v>
@@ -2239,10 +2254,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="32" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B60" s="35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C60" s="29">
         <v>35</v>
@@ -2250,7 +2265,7 @@
     </row>
     <row r="61" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="23" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B61" s="23">
         <f>B$36+SUMPRODUCT(SUMIF($B$40:$B$60,$L$1,$C$40:$C$60))+SUMPRODUCT(SUMIF($B$40:$B$60,$L$3,$C$40:$C$60))*0.5</f>
@@ -2264,32 +2279,32 @@
     <row r="62" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="64" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="18" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B64" s="10"/>
     </row>
     <row r="65" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B65" s="36" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B66" s="36" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B67" s="36" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>